<commit_message>
Update Use types with new naming convention
Updated several .csv files to change naming references to align with CEA standards.

Co-Authored-By: Mar-Ges <73158684+mar-ges@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/cea/databases/DE/archetypes/use_types/USE_TYPE_PROPERTIES.xlsx
+++ b/cea/databases/DE/archetypes/use_types/USE_TYPE_PROPERTIES.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ge38yoz\2024-02-18_DE\archetypes\use_types\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Geske\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8FC8F6-B17C-434C-9DB0-C60981C4A61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="INDOOR_COMFORT" sheetId="1" r:id="rId1"/>
     <sheet name="INTERNAL_LOADS" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t>code</t>
   </si>
@@ -60,36 +59,6 @@
     <t>RH_max_pc</t>
   </si>
   <si>
-    <t>D_EFH</t>
-  </si>
-  <si>
-    <t>D_MFH</t>
-  </si>
-  <si>
-    <t>D_SENIOR</t>
-  </si>
-  <si>
-    <t>D1_EINZELBUERO</t>
-  </si>
-  <si>
-    <t>D2_BUERO</t>
-  </si>
-  <si>
-    <t>D4_SITZUNG</t>
-  </si>
-  <si>
-    <t>D6_KAUFHAUS</t>
-  </si>
-  <si>
-    <t>D8_KITA</t>
-  </si>
-  <si>
-    <t>D8_SCHULE</t>
-  </si>
-  <si>
-    <t>D13_RESTAURANT</t>
-  </si>
-  <si>
     <t>MULTI_RES</t>
   </si>
   <si>
@@ -184,12 +153,24 @@
   </si>
   <si>
     <t>Ev_kWveh</t>
+  </si>
+  <si>
+    <t>SENIOR_RES</t>
+  </si>
+  <si>
+    <t>OFFICE_1P</t>
+  </si>
+  <si>
+    <t>SEMINAR</t>
+  </si>
+  <si>
+    <t>KINDERGARDEN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -376,7 +357,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -600,14 +581,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView zoomScale="130" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34:C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
@@ -648,7 +629,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="15">
         <v>26</v>
@@ -673,8 +654,8 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>9</v>
+      <c r="A3" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="B3" s="16">
         <v>26</v>
@@ -699,8 +680,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>10</v>
+      <c r="A4" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="B4" s="16">
         <v>26</v>
@@ -725,8 +706,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>11</v>
+      <c r="A5" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="B5" s="16">
         <v>24</v>
@@ -751,8 +732,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>12</v>
+      <c r="A6" s="10" t="s">
+        <v>11</v>
       </c>
       <c r="B6" s="16">
         <v>24</v>
@@ -777,8 +758,8 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>13</v>
+      <c r="A7" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="B7" s="16">
         <v>20</v>
@@ -803,8 +784,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>14</v>
+      <c r="A8" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="B8" s="16">
         <v>16</v>
@@ -829,8 +810,8 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>15</v>
+      <c r="A9" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="B9" s="16">
         <v>17.5</v>
@@ -855,7 +836,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="16">
@@ -881,8 +862,8 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>17</v>
+      <c r="A11" s="10" t="s">
+        <v>14</v>
       </c>
       <c r="B11" s="16">
         <v>16</v>
@@ -908,7 +889,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B12" s="7">
         <v>26</v>
@@ -920,11 +901,11 @@
         <v>28</v>
       </c>
       <c r="E12" s="8">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F12" s="9">
-        <f t="shared" ref="F12:F13" si="0">30/3.6</f>
-        <v>8.3333333333333339</v>
+        <f t="shared" ref="F12" si="0">36/3.6</f>
+        <v>10</v>
       </c>
       <c r="G12" s="9">
         <v>30</v>
@@ -935,22 +916,22 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B13" s="7">
         <v>26</v>
       </c>
       <c r="C13" s="8">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" s="7">
         <v>28</v>
       </c>
       <c r="E13" s="8">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F13" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F13" si="1">30/3.6</f>
         <v>8.3333333333333339</v>
       </c>
       <c r="G13" s="9">
@@ -961,50 +942,50 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>20</v>
+      <c r="A14" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="B14" s="7">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C14" s="8">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D14" s="7">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E14" s="8">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F14" s="9">
-        <f t="shared" ref="F14:F15" si="1">36/3.6</f>
-        <v>10</v>
+        <f>10*15/3.6</f>
+        <v>41.666666666666664</v>
       </c>
       <c r="G14" s="9">
         <v>30</v>
       </c>
       <c r="H14" s="9">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>21</v>
+      <c r="A15" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="B15" s="7">
         <v>26</v>
       </c>
       <c r="C15" s="8">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D15" s="7">
         <v>28</v>
       </c>
       <c r="E15" s="8">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F15" s="9">
-        <f t="shared" si="1"/>
+        <f>36*1000/3600</f>
         <v>10</v>
       </c>
       <c r="G15" s="9">
@@ -1016,13 +997,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B16" s="7">
         <v>26</v>
       </c>
       <c r="C16" s="8">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D16" s="7">
         <v>28</v>
@@ -1031,52 +1012,52 @@
         <v>12</v>
       </c>
       <c r="F16" s="9">
-        <f t="shared" ref="F16:F17" si="2">30/3.6</f>
-        <v>8.3333333333333339</v>
+        <f>9*10/3.6</f>
+        <v>25</v>
       </c>
       <c r="G16" s="9">
         <v>30</v>
       </c>
       <c r="H16" s="9">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B17" s="7">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C17" s="8">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D17" s="7">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E17" s="8">
         <v>12</v>
       </c>
       <c r="F17" s="9">
-        <f t="shared" si="2"/>
-        <v>8.3333333333333339</v>
+        <f>3.6*10/3.6</f>
+        <v>10</v>
       </c>
       <c r="G17" s="9">
         <v>30</v>
       </c>
       <c r="H17" s="9">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B18" s="7">
         <v>26</v>
       </c>
       <c r="C18" s="8">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D18" s="7">
         <v>28</v>
@@ -1085,35 +1066,33 @@
         <v>12</v>
       </c>
       <c r="F18" s="9">
-        <f>36/3.6</f>
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="G18" s="9">
         <v>30</v>
       </c>
       <c r="H18" s="9">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B19" s="7">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C19" s="8">
         <v>18</v>
       </c>
       <c r="D19" s="7">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E19" s="8">
         <v>12</v>
       </c>
       <c r="F19" s="9">
-        <f>10*15/3.6</f>
-        <v>41.666666666666664</v>
+        <v>0</v>
       </c>
       <c r="G19" s="9">
         <v>30</v>
@@ -1124,50 +1103,49 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B20" s="7">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="C20" s="8">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="D20" s="7">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="E20" s="8">
-        <v>12</v>
+        <v>-18</v>
       </c>
       <c r="F20" s="9">
-        <f>25/3.6</f>
-        <v>6.9444444444444446</v>
+        <v>0</v>
       </c>
       <c r="G20" s="9">
         <v>30</v>
       </c>
       <c r="H20" s="9">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B21" s="7">
         <v>26</v>
       </c>
       <c r="C21" s="8">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D21" s="7">
         <v>28</v>
       </c>
       <c r="E21" s="8">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F21" s="9">
-        <f>36*1000/3600</f>
-        <v>10</v>
+        <f>20*15/3.6</f>
+        <v>83.333333333333329</v>
       </c>
       <c r="G21" s="9">
         <v>30</v>
@@ -1178,13 +1156,13 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B22" s="7">
         <v>26</v>
       </c>
       <c r="C22" s="8">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D22" s="7">
         <v>28</v>
@@ -1193,52 +1171,52 @@
         <v>12</v>
       </c>
       <c r="F22" s="9">
-        <f>9*10/3.6</f>
-        <v>25</v>
+        <f t="shared" ref="F22:F23" si="2">36/3.6</f>
+        <v>10</v>
       </c>
       <c r="G22" s="9">
         <v>30</v>
       </c>
       <c r="H22" s="9">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B23" s="7">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C23" s="8">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D23" s="7">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E23" s="8">
         <v>12</v>
       </c>
       <c r="F23" s="9">
-        <f>3.6*10/3.6</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G23" s="9">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="H23" s="9">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B24" s="7">
         <v>26</v>
       </c>
       <c r="C24" s="8">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D24" s="7">
         <v>28</v>
@@ -1247,172 +1225,13 @@
         <v>12</v>
       </c>
       <c r="F24" s="9">
-        <v>36</v>
+        <f>30/3.6</f>
+        <v>8.3333333333333339</v>
       </c>
       <c r="G24" s="9">
         <v>30</v>
       </c>
       <c r="H24" s="9">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="7">
-        <v>28</v>
-      </c>
-      <c r="C25" s="8">
-        <v>18</v>
-      </c>
-      <c r="D25" s="7">
-        <v>28</v>
-      </c>
-      <c r="E25" s="8">
-        <v>12</v>
-      </c>
-      <c r="F25" s="9">
-        <v>0</v>
-      </c>
-      <c r="G25" s="9">
-        <v>30</v>
-      </c>
-      <c r="H25" s="9">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="7">
-        <v>2</v>
-      </c>
-      <c r="C26" s="8">
-        <v>2</v>
-      </c>
-      <c r="D26" s="7">
-        <v>2</v>
-      </c>
-      <c r="E26" s="8">
-        <v>-18</v>
-      </c>
-      <c r="F26" s="9">
-        <v>0</v>
-      </c>
-      <c r="G26" s="9">
-        <v>30</v>
-      </c>
-      <c r="H26" s="9">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="7">
-        <v>26</v>
-      </c>
-      <c r="C27" s="8">
-        <v>21</v>
-      </c>
-      <c r="D27" s="7">
-        <v>28</v>
-      </c>
-      <c r="E27" s="8">
-        <v>12</v>
-      </c>
-      <c r="F27" s="9">
-        <f>20*15/3.6</f>
-        <v>83.333333333333329</v>
-      </c>
-      <c r="G27" s="9">
-        <v>30</v>
-      </c>
-      <c r="H27" s="9">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28" s="7">
-        <v>26</v>
-      </c>
-      <c r="C28" s="8">
-        <v>21</v>
-      </c>
-      <c r="D28" s="7">
-        <v>28</v>
-      </c>
-      <c r="E28" s="8">
-        <v>12</v>
-      </c>
-      <c r="F28" s="9">
-        <f t="shared" ref="F28:F29" si="3">36/3.6</f>
-        <v>10</v>
-      </c>
-      <c r="G28" s="9">
-        <v>30</v>
-      </c>
-      <c r="H28" s="9">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" s="7">
-        <v>26</v>
-      </c>
-      <c r="C29" s="8">
-        <v>21</v>
-      </c>
-      <c r="D29" s="7">
-        <v>28</v>
-      </c>
-      <c r="E29" s="8">
-        <v>12</v>
-      </c>
-      <c r="F29" s="9">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-      <c r="G29" s="9">
-        <v>40</v>
-      </c>
-      <c r="H29" s="9">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" s="7">
-        <v>26</v>
-      </c>
-      <c r="C30" s="8">
-        <v>21</v>
-      </c>
-      <c r="D30" s="7">
-        <v>28</v>
-      </c>
-      <c r="E30" s="8">
-        <v>12</v>
-      </c>
-      <c r="F30" s="9">
-        <f>30/3.6</f>
-        <v>8.3333333333333339</v>
-      </c>
-      <c r="G30" s="9">
-        <v>30</v>
-      </c>
-      <c r="H30" s="9">
         <v>60</v>
       </c>
     </row>
@@ -1423,14 +1242,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView zoomScale="130" workbookViewId="0">
+      <selection activeCell="A11" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" style="2" customWidth="1"/>
@@ -1452,48 +1271,48 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="13">
         <v>48</v>
@@ -1536,8 +1355,8 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>9</v>
+      <c r="A3" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="B3" s="14">
         <v>35</v>
@@ -1581,7 +1400,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="B4" s="14">
         <v>35</v>
@@ -1625,7 +1444,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="B5" s="14">
         <v>14</v>
@@ -1669,7 +1488,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="14">
         <v>17</v>
@@ -1713,7 +1532,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="B7" s="14">
         <v>2</v>
@@ -1757,7 +1576,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="14">
         <v>5</v>
@@ -1801,7 +1620,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="B9" s="14">
         <v>3</v>
@@ -1889,7 +1708,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B11" s="14">
         <v>1.2</v>
@@ -1932,11 +1751,11 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>18</v>
+      <c r="A12" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="B12" s="11">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C12" s="11">
         <v>70</v>
@@ -1950,7 +1769,7 @@
       <c r="F12" s="11">
         <v>2.7</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="11">
         <v>0</v>
       </c>
       <c r="H12" s="9">
@@ -1960,7 +1779,7 @@
         <v>40</v>
       </c>
       <c r="J12" s="11">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="K12" s="9">
         <v>0</v>
@@ -1977,22 +1796,23 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B13" s="11">
-        <v>50</v>
-      </c>
-      <c r="C13" s="9">
+        <v>8</v>
+      </c>
+      <c r="C13" s="11">
         <v>70</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="11">
         <v>80</v>
       </c>
-      <c r="E13" s="9">
-        <v>8</v>
-      </c>
-      <c r="F13" s="9">
-        <v>2.7</v>
+      <c r="E13" s="11">
+        <v>2</v>
+      </c>
+      <c r="F13" s="11">
+        <f>9.3+24</f>
+        <v>33.299999999999997</v>
       </c>
       <c r="G13" s="11">
         <v>0</v>
@@ -2001,10 +1821,10 @@
         <v>0</v>
       </c>
       <c r="I13" s="11">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="J13" s="11">
-        <v>160</v>
+        <v>30</v>
       </c>
       <c r="K13" s="9">
         <v>0</v>
@@ -2020,41 +1840,41 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>20</v>
+      <c r="A14" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="B14" s="11">
         <v>15</v>
       </c>
       <c r="C14" s="11">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="D14" s="11">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="E14" s="11">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F14" s="11">
-        <v>2.7</v>
+        <v>10.8</v>
       </c>
       <c r="G14" s="11">
-        <v>0</v>
+        <v>16.5</v>
       </c>
       <c r="H14" s="9">
         <v>0</v>
       </c>
       <c r="I14" s="11">
-        <v>40</v>
+        <v>3</v>
       </c>
       <c r="J14" s="11">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="K14" s="9">
         <v>0</v>
       </c>
       <c r="L14" s="9">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="M14" s="9">
         <v>0</v>
@@ -2065,10 +1885,11 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B15" s="11">
-        <v>14</v>
+        <f>15*0.43+3*0.01+5*0.56</f>
+        <v>9.2800000000000011</v>
       </c>
       <c r="C15" s="11">
         <v>70</v>
@@ -2077,10 +1898,12 @@
         <v>80</v>
       </c>
       <c r="E15" s="11">
-        <v>7</v>
+        <f>0.43*4+0.01*7+0.56*20</f>
+        <v>12.990000000000002</v>
       </c>
       <c r="F15" s="11">
-        <v>15.9</v>
+        <f>0.43*4.5+0.01*15.9+0.56*15.9</f>
+        <v>10.998000000000001</v>
       </c>
       <c r="G15" s="11">
         <v>0</v>
@@ -2089,16 +1912,18 @@
         <v>0</v>
       </c>
       <c r="I15" s="11">
-        <v>3</v>
+        <f>0.43*60+0.01*0+0.56*0</f>
+        <v>25.8</v>
       </c>
       <c r="J15" s="11">
-        <v>60</v>
+        <f>I15*4</f>
+        <v>103.2</v>
       </c>
       <c r="K15" s="9">
         <v>0</v>
       </c>
       <c r="L15" s="9">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M15" s="9">
         <v>0</v>
@@ -2109,23 +1934,22 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B16" s="11">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C16" s="11">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="D16" s="11">
-        <v>80</v>
+        <v>280</v>
       </c>
       <c r="E16" s="11">
         <v>2</v>
       </c>
       <c r="F16" s="11">
-        <f>9.3+24</f>
-        <v>33.299999999999997</v>
+        <v>9.9</v>
       </c>
       <c r="G16" s="11">
         <v>0</v>
@@ -2134,10 +1958,10 @@
         <v>0</v>
       </c>
       <c r="I16" s="11">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="J16" s="11">
-        <v>30</v>
+        <v>180</v>
       </c>
       <c r="K16" s="9">
         <v>0</v>
@@ -2154,10 +1978,10 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B17" s="11">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C17" s="11">
         <v>70</v>
@@ -2169,8 +1993,7 @@
         <v>2</v>
       </c>
       <c r="F17" s="11">
-        <f>9.3+12</f>
-        <v>21.3</v>
+        <v>11.3</v>
       </c>
       <c r="G17" s="11">
         <v>0</v>
@@ -2179,13 +2002,13 @@
         <v>0</v>
       </c>
       <c r="I17" s="11">
-        <v>2</v>
+        <v>120</v>
       </c>
       <c r="J17" s="11">
-        <v>30</v>
+        <v>360</v>
       </c>
       <c r="K17" s="9">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L17" s="9">
         <v>0</v>
@@ -2199,34 +2022,34 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B18" s="11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C18" s="11">
         <v>70</v>
       </c>
       <c r="D18" s="11">
-        <v>80</v>
-      </c>
-      <c r="E18" s="11">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="E18" s="12">
+        <v>0</v>
       </c>
       <c r="F18" s="11">
-        <v>6.9</v>
+        <v>6.6</v>
       </c>
       <c r="G18" s="11">
         <v>0</v>
       </c>
-      <c r="H18" s="9">
-        <v>0</v>
+      <c r="H18" s="11">
+        <v>100</v>
       </c>
       <c r="I18" s="11">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="J18" s="11">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="K18" s="9">
         <v>0</v>
@@ -2243,40 +2066,40 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B19" s="11">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C19" s="11">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="D19" s="11">
-        <v>170</v>
+        <v>0</v>
       </c>
       <c r="E19" s="11">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F19" s="11">
-        <v>10.8</v>
+        <v>2.9</v>
       </c>
       <c r="G19" s="11">
-        <v>16.5</v>
+        <v>0</v>
       </c>
       <c r="H19" s="9">
         <v>0</v>
       </c>
       <c r="I19" s="11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J19" s="11">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="K19" s="9">
         <v>0</v>
       </c>
       <c r="L19" s="9">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="M19" s="9">
         <v>0</v>
@@ -2287,22 +2110,22 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B20" s="11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C20" s="11">
         <v>70</v>
       </c>
       <c r="D20" s="11">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="E20" s="11">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F20" s="11">
-        <v>14</v>
+        <v>5.7</v>
       </c>
       <c r="G20" s="11">
         <v>0</v>
@@ -2311,13 +2134,13 @@
         <v>0</v>
       </c>
       <c r="I20" s="11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J20" s="11">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="K20" s="9">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L20" s="9">
         <v>0</v>
@@ -2331,45 +2154,43 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B21" s="11">
-        <f>15*0.43+3*0.01+5*0.56</f>
-        <v>9.2800000000000011</v>
+        <v>15</v>
       </c>
       <c r="C21" s="11">
+        <f>C15</f>
         <v>70</v>
       </c>
       <c r="D21" s="11">
+        <f>D15</f>
         <v>80</v>
       </c>
       <c r="E21" s="11">
-        <f>0.43*4+0.01*7+0.56*20</f>
-        <v>12.990000000000002</v>
+        <v>20</v>
       </c>
       <c r="F21" s="11">
-        <f>0.43*4.5+0.01*15.9+0.56*15.9</f>
-        <v>10.998000000000001</v>
+        <v>16.2</v>
       </c>
       <c r="G21" s="11">
-        <v>0</v>
+        <f>G14</f>
+        <v>16.5</v>
       </c>
       <c r="H21" s="9">
         <v>0</v>
       </c>
       <c r="I21" s="11">
-        <f>0.43*60+0.01*0+0.56*0</f>
-        <v>25.8</v>
+        <v>3</v>
       </c>
       <c r="J21" s="11">
-        <f>I21*4</f>
-        <v>103.2</v>
+        <v>60</v>
       </c>
       <c r="K21" s="9">
         <v>0</v>
       </c>
       <c r="L21" s="9">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="M21" s="9">
         <v>0</v>
@@ -2380,34 +2201,34 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B22" s="11">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C22" s="11">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="D22" s="11">
-        <v>280</v>
+        <v>80</v>
       </c>
       <c r="E22" s="11">
+        <v>7</v>
+      </c>
+      <c r="F22" s="11">
+        <v>10.8</v>
+      </c>
+      <c r="G22" s="11">
+        <v>0</v>
+      </c>
+      <c r="H22" s="9">
+        <v>0</v>
+      </c>
+      <c r="I22" s="11">
         <v>2</v>
       </c>
-      <c r="F22" s="11">
-        <v>9.9</v>
-      </c>
-      <c r="G22" s="11">
-        <v>0</v>
-      </c>
-      <c r="H22" s="9">
-        <v>0</v>
-      </c>
-      <c r="I22" s="11">
-        <v>60</v>
-      </c>
       <c r="J22" s="11">
-        <v>180</v>
+        <v>30</v>
       </c>
       <c r="K22" s="9">
         <v>0</v>
@@ -2424,10 +2245,10 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B23" s="11">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C23" s="11">
         <v>70</v>
@@ -2439,7 +2260,7 @@
         <v>2</v>
       </c>
       <c r="F23" s="11">
-        <v>11.3</v>
+        <v>6.9</v>
       </c>
       <c r="G23" s="11">
         <v>0</v>
@@ -2448,10 +2269,10 @@
         <v>0</v>
       </c>
       <c r="I23" s="11">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="J23" s="11">
-        <v>360</v>
+        <v>0</v>
       </c>
       <c r="K23" s="9">
         <v>0</v>
@@ -2468,34 +2289,34 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B24" s="11">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C24" s="11">
         <v>70</v>
       </c>
       <c r="D24" s="11">
-        <v>0</v>
-      </c>
-      <c r="E24" s="12">
-        <v>0</v>
+        <v>80</v>
+      </c>
+      <c r="E24" s="11">
+        <v>4</v>
       </c>
       <c r="F24" s="11">
-        <v>6.6</v>
+        <v>12.5</v>
       </c>
       <c r="G24" s="11">
         <v>0</v>
       </c>
-      <c r="H24" s="11">
-        <v>100</v>
+      <c r="H24" s="9">
+        <v>0</v>
       </c>
       <c r="I24" s="11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J24" s="11">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K24" s="9">
         <v>0</v>
@@ -2507,273 +2328,6 @@
         <v>0</v>
       </c>
       <c r="N24" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="11">
-        <v>0</v>
-      </c>
-      <c r="C25" s="11">
-        <v>35</v>
-      </c>
-      <c r="D25" s="11">
-        <v>0</v>
-      </c>
-      <c r="E25" s="11">
-        <v>1</v>
-      </c>
-      <c r="F25" s="11">
-        <v>2.9</v>
-      </c>
-      <c r="G25" s="11">
-        <v>0</v>
-      </c>
-      <c r="H25" s="9">
-        <v>0</v>
-      </c>
-      <c r="I25" s="11">
-        <v>0</v>
-      </c>
-      <c r="J25" s="11">
-        <v>0</v>
-      </c>
-      <c r="K25" s="9">
-        <v>0</v>
-      </c>
-      <c r="L25" s="9">
-        <v>0</v>
-      </c>
-      <c r="M25" s="9">
-        <v>0</v>
-      </c>
-      <c r="N25" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="11">
-        <v>0</v>
-      </c>
-      <c r="C26" s="11">
-        <v>70</v>
-      </c>
-      <c r="D26" s="11">
-        <v>0</v>
-      </c>
-      <c r="E26" s="11">
-        <v>0</v>
-      </c>
-      <c r="F26" s="11">
-        <v>5.7</v>
-      </c>
-      <c r="G26" s="11">
-        <v>0</v>
-      </c>
-      <c r="H26" s="9">
-        <v>0</v>
-      </c>
-      <c r="I26" s="11">
-        <v>0</v>
-      </c>
-      <c r="J26" s="11">
-        <v>0</v>
-      </c>
-      <c r="K26" s="9">
-        <v>100</v>
-      </c>
-      <c r="L26" s="9">
-        <v>0</v>
-      </c>
-      <c r="M26" s="9">
-        <v>0</v>
-      </c>
-      <c r="N26" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="11">
-        <v>15</v>
-      </c>
-      <c r="C27" s="11">
-        <f>C21</f>
-        <v>70</v>
-      </c>
-      <c r="D27" s="11">
-        <f>D21</f>
-        <v>80</v>
-      </c>
-      <c r="E27" s="11">
-        <v>20</v>
-      </c>
-      <c r="F27" s="11">
-        <v>16.2</v>
-      </c>
-      <c r="G27" s="11">
-        <f>G19</f>
-        <v>16.5</v>
-      </c>
-      <c r="H27" s="9">
-        <v>0</v>
-      </c>
-      <c r="I27" s="11">
-        <v>3</v>
-      </c>
-      <c r="J27" s="11">
-        <v>60</v>
-      </c>
-      <c r="K27" s="9">
-        <v>0</v>
-      </c>
-      <c r="L27" s="9">
-        <v>0</v>
-      </c>
-      <c r="M27" s="9">
-        <v>0</v>
-      </c>
-      <c r="N27" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28" s="11">
-        <v>3</v>
-      </c>
-      <c r="C28" s="11">
-        <v>70</v>
-      </c>
-      <c r="D28" s="11">
-        <v>80</v>
-      </c>
-      <c r="E28" s="11">
-        <v>7</v>
-      </c>
-      <c r="F28" s="11">
-        <v>10.8</v>
-      </c>
-      <c r="G28" s="11">
-        <v>0</v>
-      </c>
-      <c r="H28" s="9">
-        <v>0</v>
-      </c>
-      <c r="I28" s="11">
-        <v>2</v>
-      </c>
-      <c r="J28" s="11">
-        <v>30</v>
-      </c>
-      <c r="K28" s="9">
-        <v>0</v>
-      </c>
-      <c r="L28" s="9">
-        <v>0</v>
-      </c>
-      <c r="M28" s="9">
-        <v>0</v>
-      </c>
-      <c r="N28" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" s="11">
-        <v>5</v>
-      </c>
-      <c r="C29" s="11">
-        <v>70</v>
-      </c>
-      <c r="D29" s="11">
-        <v>80</v>
-      </c>
-      <c r="E29" s="11">
-        <v>2</v>
-      </c>
-      <c r="F29" s="11">
-        <v>6.9</v>
-      </c>
-      <c r="G29" s="11">
-        <v>0</v>
-      </c>
-      <c r="H29" s="9">
-        <v>0</v>
-      </c>
-      <c r="I29" s="11">
-        <v>0</v>
-      </c>
-      <c r="J29" s="11">
-        <v>0</v>
-      </c>
-      <c r="K29" s="9">
-        <v>0</v>
-      </c>
-      <c r="L29" s="9">
-        <v>0</v>
-      </c>
-      <c r="M29" s="9">
-        <v>0</v>
-      </c>
-      <c r="N29" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" s="11">
-        <v>10</v>
-      </c>
-      <c r="C30" s="11">
-        <v>70</v>
-      </c>
-      <c r="D30" s="11">
-        <v>80</v>
-      </c>
-      <c r="E30" s="11">
-        <v>4</v>
-      </c>
-      <c r="F30" s="11">
-        <v>12.5</v>
-      </c>
-      <c r="G30" s="11">
-        <v>0</v>
-      </c>
-      <c r="H30" s="9">
-        <v>0</v>
-      </c>
-      <c r="I30" s="11">
-        <v>2</v>
-      </c>
-      <c r="J30" s="11">
-        <v>30</v>
-      </c>
-      <c r="K30" s="9">
-        <v>0</v>
-      </c>
-      <c r="L30" s="9">
-        <v>0</v>
-      </c>
-      <c r="M30" s="9">
-        <v>0</v>
-      </c>
-      <c r="N30" s="9">
         <v>0</v>
       </c>
     </row>
@@ -2784,6 +2338,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C4119BA2A2C9A34A9ABDCD539C093B2A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2036187cb88b360b5a6de576d0a5f2f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="be70d004-d1e5-4317-a402-eff109a4a2bb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e63961df46f11abd186e13992df6f3c7" ns3:_="">
     <xsd:import namespace="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
@@ -2953,35 +2522,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02AC8DD-FE6B-486F-A4E4-4D415B112715}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3003,9 +2547,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02AC8DD-FE6B-486F-A4E4-4D415B112715}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update warmwater and setpoint
With latest BDEW values (42 % of 121 ldp) and increase to 20,9 °C (statista)
</commit_message>
<xml_diff>
--- a/cea/databases/DE/archetypes/use_types/USE_TYPE_PROPERTIES.xlsx
+++ b/cea/databases/DE/archetypes/use_types/USE_TYPE_PROPERTIES.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Geske\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ge38yoz\CityEnergyAnalystFork\cea\databases\DE\archetypes\use_types\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32E95E9-0404-442E-AE1E-D309CBD20861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INDOOR_COMFORT" sheetId="1" r:id="rId1"/>
     <sheet name="INTERNAL_LOADS" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -24,8 +25,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -170,7 +169,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -305,7 +304,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -353,6 +352,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -581,11 +583,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34:C35"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,13 +637,13 @@
         <v>26</v>
       </c>
       <c r="C2" s="13">
-        <v>20</v>
+        <v>20.9</v>
       </c>
       <c r="D2" s="13">
         <v>32</v>
       </c>
       <c r="E2" s="13">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F2" s="13">
         <v>8.3000000000000007</v>
@@ -660,14 +662,14 @@
       <c r="B3" s="16">
         <v>26</v>
       </c>
-      <c r="C3" s="14">
-        <v>20</v>
+      <c r="C3" s="13">
+        <v>20.9</v>
       </c>
       <c r="D3" s="14">
         <v>32</v>
       </c>
       <c r="E3" s="14">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F3" s="14">
         <v>8.3000000000000007</v>
@@ -686,14 +688,14 @@
       <c r="B4" s="16">
         <v>26</v>
       </c>
-      <c r="C4" s="14">
-        <v>20</v>
+      <c r="C4" s="13">
+        <v>20.9</v>
       </c>
       <c r="D4" s="14">
         <v>32</v>
       </c>
       <c r="E4" s="14">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F4" s="14">
         <v>8.3000000000000007</v>
@@ -1242,11 +1244,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView zoomScale="130" workbookViewId="0">
-      <selection activeCell="A11" sqref="A2:A11"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1335,8 +1337,8 @@
       <c r="H2" s="13">
         <v>0</v>
       </c>
-      <c r="I2" s="13">
-        <v>11.6</v>
+      <c r="I2" s="17">
+        <v>50.82</v>
       </c>
       <c r="J2" s="13">
         <v>115.4</v>
@@ -1379,8 +1381,8 @@
       <c r="H3" s="14">
         <v>0</v>
       </c>
-      <c r="I3" s="13">
-        <v>11.6</v>
+      <c r="I3" s="17">
+        <v>50.82</v>
       </c>
       <c r="J3" s="13">
         <v>115.4</v>
@@ -1423,8 +1425,8 @@
       <c r="H4" s="14">
         <v>0</v>
       </c>
-      <c r="I4" s="13">
-        <v>11.6</v>
+      <c r="I4" s="17">
+        <v>50.82</v>
       </c>
       <c r="J4" s="13">
         <v>115.4</v>
@@ -2338,21 +2340,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C4119BA2A2C9A34A9ABDCD539C093B2A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2036187cb88b360b5a6de576d0a5f2f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="be70d004-d1e5-4317-a402-eff109a4a2bb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e63961df46f11abd186e13992df6f3c7" ns3:_="">
     <xsd:import namespace="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
@@ -2522,10 +2509,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02AC8DD-FE6B-486F-A4E4-4D415B112715}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2547,19 +2559,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02AC8DD-FE6B-486F-A4E4-4D415B112715}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>